<commit_message>
Finally, the roster excel can be generated from the template.xlsx
</commit_message>
<xml_diff>
--- a/server/testing/template.xlsx
+++ b/server/testing/template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20372"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\cstsang\workspace\rosterWeb_react_node\server\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Roy.DESKTOP-80CAPLI\workspace\rosterWeb_react_node\server\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889B4739-CF17-46E6-92CD-75F059C69A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="4200" windowWidth="23250" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2066" yWindow="4195" windowWidth="23253" windowHeight="12346"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,15 +188,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="\+#0.##;\-#0.##"/>
+    <numFmt numFmtId="164" formatCode="\+#0.##;\-#0.##"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -237,7 +236,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -263,17 +262,24 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
       <charset val="136"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -449,7 +455,7 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -545,14 +551,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="一般 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="一般 3" xfId="1"/>
+    <cellStyle name="一般 4" xfId="2"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -678,23 +684,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -730,23 +719,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -922,36 +894,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.65"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="21" width="3.125" customWidth="1"/>
-    <col min="22" max="22" width="2.875" customWidth="1"/>
-    <col min="23" max="32" width="3.125" customWidth="1"/>
-    <col min="33" max="33" width="10.125" customWidth="1"/>
-    <col min="34" max="34" width="8.875" customWidth="1"/>
-    <col min="35" max="35" width="8.25" customWidth="1"/>
-    <col min="36" max="36" width="8.625" customWidth="1"/>
-    <col min="37" max="37" width="7.875" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
+    <col min="2" max="21" width="3.09765625" customWidth="1"/>
+    <col min="22" max="22" width="2.8984375" customWidth="1"/>
+    <col min="23" max="32" width="3.09765625" customWidth="1"/>
+    <col min="33" max="33" width="10.09765625" customWidth="1"/>
+    <col min="34" max="34" width="8.8984375" customWidth="1"/>
+    <col min="35" max="35" width="8.19921875" customWidth="1"/>
+    <col min="36" max="36" width="8.59765625" customWidth="1"/>
+    <col min="37" max="37" width="7.8984375" customWidth="1"/>
     <col min="38" max="38" width="4.5" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="5.625" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="5.59765625" hidden="1" customWidth="1"/>
     <col min="40" max="41" width="4.5" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="3.375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="6.25" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="3.3984375" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="6.19921875" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" ht="18.2">
       <c r="A1" s="2"/>
       <c r="B1" s="31" t="s">
         <v>0</v>
@@ -998,7 +970,7 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="17.55">
       <c r="A2" s="1"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1045,7 +1017,7 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43">
       <c r="A4" s="19" t="s">
         <v>30</v>
       </c>
@@ -1092,7 +1064,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="15.85" customHeight="1">
       <c r="A5" s="19" t="s">
         <v>31</v>
       </c>
@@ -1145,7 +1117,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="31.3">
       <c r="A6" s="41" t="s">
         <v>50</v>
       </c>
@@ -1210,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43">
       <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
@@ -1246,7 +1218,7 @@
       <c r="AE7" s="10"/>
       <c r="AF7" s="10"/>
     </row>
-    <row r="8" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" ht="17.55">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
@@ -1280,7 +1252,7 @@
       <c r="AA8" s="30"/>
       <c r="AB8" s="30"/>
     </row>
-    <row r="9" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" ht="17.55">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -1314,7 +1286,7 @@
       <c r="AA9" s="30"/>
       <c r="AB9" s="30"/>
     </row>
-    <row r="10" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" ht="17.55">
       <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
@@ -1346,7 +1318,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" ht="17.55">
       <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
@@ -1384,7 +1356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" ht="17.55">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
@@ -1420,7 +1392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" ht="17.55">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" ht="17.55">
       <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" ht="17.55">
       <c r="A15" s="16" t="s">
         <v>15</v>
       </c>
@@ -1524,7 +1496,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" ht="17.55">
       <c r="A16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1556,7 +1528,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="17.55">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
@@ -1588,7 +1560,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1638,76 +1610,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ13"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="N13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.65"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:43" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" ht="17.55">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1801,12 +1773,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.65"/>
   <sheetData/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>